<commit_message>
Added text in .xls and .xlsx on 3rd sheet and added tests
</commit_message>
<xml_diff>
--- a/src/main/resources/files/1.xlsx
+++ b/src/main/resources/files/1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="22995" windowHeight="9780"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="22995" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>This is B4 cell</t>
   </si>
   <si>
     <t>This is .xlsx file</t>
+  </si>
+  <si>
+    <t>Something on 3rd sheet</t>
   </si>
 </sst>
 </file>
@@ -356,7 +359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -391,12 +394,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="3:3">
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>